<commit_message>
Customized pension and savings categories
</commit_message>
<xml_diff>
--- a/expense_presets.xlsx
+++ b/expense_presets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA136117-D54B-484C-BD0D-4DDFEEEF3C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDB92F2-6372-4971-86F0-66913554C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
   </bookViews>
   <sheets>
     <sheet name="mainoptions" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="breakdowns" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -520,7 +521,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="B1">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -545,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -556,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
@@ -578,7 +579,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>2480</v>
+        <v>2484</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -593,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE86E16-34BF-4FB6-B40F-42204A9170B8}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -722,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EAC4F3-A43D-4AC6-96B8-43711A178B2D}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,10 +755,10 @@
         <v>0</v>
       </c>
       <c r="I1">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="J1">
-        <v>85</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -786,10 +787,10 @@
         <v>65</v>
       </c>
       <c r="I2">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="J2">
-        <v>115</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -818,10 +819,10 @@
         <v>75</v>
       </c>
       <c r="I3">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="J3">
-        <v>135</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -850,10 +851,10 @@
         <v>110</v>
       </c>
       <c r="I4">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="J4">
-        <v>165</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -882,10 +883,10 @@
         <v>140</v>
       </c>
       <c r="I5">
-        <v>205</v>
+        <v>10</v>
       </c>
       <c r="J5">
-        <v>205</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -914,10 +915,10 @@
         <v>320</v>
       </c>
       <c r="I6">
-        <v>275</v>
+        <v>25</v>
       </c>
       <c r="J6">
-        <v>275</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Layout and tooltips update.
</commit_message>
<xml_diff>
--- a/expense_presets.xlsx
+++ b/expense_presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDB92F2-6372-4971-86F0-66913554C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E760AC3-BEDA-4701-8471-39E898FE2FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
   </bookViews>
   <sheets>
     <sheet name="mainoptions" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="breakdowns" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,9 +76,6 @@
     <t>Essentials for Living</t>
   </si>
   <si>
-    <t>All Other (Education, Insurance, Social and Financial Services)</t>
-  </si>
-  <si>
     <t>Enough for typical expenditure for a UK household and savings and pensions for this lifestyle.</t>
   </si>
   <si>
@@ -107,19 +103,7 @@
     <t>Including car purchase and running costs, public transport, and flights</t>
   </si>
   <si>
-    <t>Including mobile phone and internet services and devices, other electronic devices</t>
-  </si>
-  <si>
     <t>Including hobbies, leisure activities, holiday expenses, restaurants and hotels</t>
-  </si>
-  <si>
-    <t>Including education costs, insurance, child and adult social care, financial services</t>
-  </si>
-  <si>
-    <t>Percentage of expenses to save for a pension</t>
-  </si>
-  <si>
-    <t>How many months needed to save one month of expenses</t>
   </si>
   <si>
     <t>Enough for essentials for living including:
@@ -164,6 +148,21 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Including education costs, insurance, social care, financial services</t>
+  </si>
+  <si>
+    <t>Including mobile phone and internet services, and related electronic devices</t>
+  </si>
+  <si>
+    <t>All Other</t>
+  </si>
+  <si>
+    <t>Percentage of income to save (after pension contribution deducted)</t>
+  </si>
+  <si>
+    <t>Percentage of income to save for a pension</t>
   </si>
 </sst>
 </file>
@@ -538,7 +537,7 @@
         <v>1008</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -549,7 +548,7 @@
         <v>1368</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -560,29 +559,29 @@
         <v>1608</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1980</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>2484</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE86E16-34BF-4FB6-B40F-42204A9170B8}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,10 +619,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,10 +641,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,10 +663,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,18 +677,18 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,7 +699,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EAC4F3-A43D-4AC6-96B8-43711A178B2D}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Lifetime expenses initial commit
</commit_message>
<xml_diff>
--- a/expense_presets.xlsx
+++ b/expense_presets.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05C05D-FB12-453F-8972-F31980DB7E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7134276-8390-4F08-9694-01119FE1F2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
   </bookViews>
   <sheets>
     <sheet name="mainoptions" sheetId="6" r:id="rId1"/>
     <sheet name="categories" sheetId="7" r:id="rId2"/>
     <sheet name="breakdowns" sheetId="1" r:id="rId3"/>
+    <sheet name="lifetime_categories" sheetId="8" r:id="rId4"/>
+    <sheet name="lifetime_breakdowns" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Housing</t>
   </si>
@@ -156,13 +158,34 @@
     <t>Including mobile phone and internet services, and related electronic devices</t>
   </si>
   <si>
-    <t>All Other</t>
-  </si>
-  <si>
     <t>Percentage of income to save (after pension contribution deducted)</t>
   </si>
   <si>
     <t>Percentage of income to save for a pension</t>
+  </si>
+  <si>
+    <t>First house downpayment</t>
+  </si>
+  <si>
+    <t>All other</t>
+  </si>
+  <si>
+    <t>Pre-school childcare</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Childcare</t>
+  </si>
+  <si>
+    <t>Deposit for buying a first house</t>
+  </si>
+  <si>
+    <t>Monthly payments for childcare, over and above government-provided childcare hours of 15-30 hours/week during term times for ages 3 and over</t>
+  </si>
+  <si>
+    <t>Childcareyears</t>
   </si>
 </sst>
 </file>
@@ -523,13 +546,13 @@
       <selection activeCell="D1" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -540,7 +563,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -551,7 +574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -562,7 +585,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -573,7 +596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -594,16 +617,16 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -625,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -636,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -647,7 +670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -658,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -669,7 +692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -680,9 +703,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -691,7 +714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -699,10 +722,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -710,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -722,13 +745,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EAC4F3-A43D-4AC6-96B8-43711A178B2D}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>500</v>
       </c>
@@ -760,7 +783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>550</v>
       </c>
@@ -792,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>600</v>
       </c>
@@ -824,7 +847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>650</v>
       </c>
@@ -856,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>800</v>
       </c>
@@ -888,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>900</v>
       </c>
@@ -918,6 +941,138 @@
       </c>
       <c r="J6">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172CA4B3-0B56-4B66-B82E-559933881C85}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C266B24-0827-4F15-963E-CC5A461E8F61}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>20000</v>
+      </c>
+      <c r="B1">
+        <v>600</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20000</v>
+      </c>
+      <c r="B2">
+        <v>600</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20000</v>
+      </c>
+      <c r="B3">
+        <v>600</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>20000</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>50000</v>
+      </c>
+      <c r="B6">
+        <v>1200</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate pages for lifetime expenses and retirement
</commit_message>
<xml_diff>
--- a/expense_presets.xlsx
+++ b/expense_presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93531E90-7ECE-42D1-A94A-7174894E3865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461C093B-4174-41A5-9D0F-0926156D06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
   </bookViews>
   <sheets>
     <sheet name="mainoptions" sheetId="6" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Typical Household</t>
   </si>
   <si>
-    <t>Rent or mortgage payments and council tax</t>
-  </si>
-  <si>
     <t>Food and drink, excluding eating out</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Childcareyears</t>
+  </si>
+  <si>
+    <t>Rent or mortgage payments</t>
   </si>
 </sst>
 </file>
@@ -542,17 +542,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D60125-C1C9-4727-93AC-10BE63E2B03B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -560,10 +560,10 @@
         <v>1241</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -571,10 +571,10 @@
         <v>1636</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -582,10 +582,10 @@
         <v>1988</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -596,7 +596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -616,17 +616,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE86E16-34BF-4FB6-B40F-42204A9170B8}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,43 +634,43 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -678,21 +678,21 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -700,21 +700,21 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -722,10 +722,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -733,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -749,9 +749,9 @@
       <selection activeCell="K1" sqref="K1:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>500</v>
       </c>
@@ -787,7 +787,7 @@
         <v>1240.7407407407406</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>550</v>
       </c>
@@ -823,7 +823,7 @@
         <v>1635.8024691358023</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>600</v>
       </c>
@@ -859,7 +859,7 @@
         <v>1987.6543209876543</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>650</v>
       </c>
@@ -895,7 +895,7 @@
         <v>2592.5925925925926</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>800</v>
       </c>
@@ -931,7 +931,7 @@
         <v>3240.7407407407404</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>900</v>
       </c>
@@ -976,42 +976,42 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1027,9 +1027,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>20000</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20000</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20000</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20000</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20000</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50000</v>
       </c>

</xml_diff>

<commit_message>
Update to new financial year. Text updates
</commit_message>
<xml_diff>
--- a/expense_presets.xlsx
+++ b/expense_presets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461C093B-4174-41A5-9D0F-0926156D06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A183E0D-6ACD-4AC7-89DC-FD9F00495F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
+    <workbookView xWindow="1416" yWindow="0" windowWidth="21624" windowHeight="11172" activeTab="2" xr2:uid="{1DCFFA5F-B13D-45C5-9C54-849CC995150D}"/>
   </bookViews>
   <sheets>
     <sheet name="mainoptions" sheetId="6" r:id="rId1"/>
@@ -616,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE86E16-34BF-4FB6-B40F-42204A9170B8}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -743,15 +743,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EAC4F3-A43D-4AC6-96B8-43711A178B2D}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>500</v>
       </c>
@@ -782,12 +782,8 @@
       <c r="J1">
         <v>10</v>
       </c>
-      <c r="K1">
-        <f>SUM(A1:H1)/(0.9*0.9)</f>
-        <v>1240.7407407407406</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>550</v>
       </c>
@@ -818,12 +814,8 @@
       <c r="J2">
         <v>10</v>
       </c>
-      <c r="K2">
-        <f t="shared" ref="K2:K5" si="0">SUM(A2:H2)/(0.9*0.9)</f>
-        <v>1635.8024691358023</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>600</v>
       </c>
@@ -854,12 +846,8 @@
       <c r="J3">
         <v>10</v>
       </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>1987.6543209876543</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>650</v>
       </c>
@@ -890,12 +878,8 @@
       <c r="J4">
         <v>10</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>2592.5925925925926</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>800</v>
       </c>
@@ -926,14 +910,10 @@
       <c r="J5">
         <v>10</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>3240.7407407407404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="B6">
         <v>325</v>

</xml_diff>